<commit_message>
Add comprehensive PDF template, individual/group/guide views, and improved PDF formatting
</commit_message>
<xml_diff>
--- a/Class_data1.xlsx
+++ b/Class_data1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/BB57047F4F84A072/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/732f7a05136b9fb7/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1BCCBF4-6CBA-491C-9791-6B14E991CFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{66BB1E5F-7465-44D4-929C-717B7A7A4710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94040B6B-D9EA-45DC-890E-8A631FAE0F36}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B586B2C6-B6DD-45C6-96B4-0AA41D419F1B}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve"> S.No</t>
   </si>
@@ -111,13 +109,31 @@
   </si>
   <si>
     <t xml:space="preserve">Prof. Rajshekhar </t>
+  </si>
+  <si>
+    <t>Ningamma</t>
+  </si>
+  <si>
+    <t>3GN22CS059</t>
+  </si>
+  <si>
+    <t>Kanaka</t>
+  </si>
+  <si>
+    <t>3GN22CS037</t>
+  </si>
+  <si>
+    <t>Akshata</t>
+  </si>
+  <si>
+    <t>3GN22CS006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB51114-A1B2-43E6-85E4-754F474A28F3}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -548,7 +564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -577,7 +593,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -606,7 +622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -633,6 +649,93 @@
       </c>
       <c r="I5">
         <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>47</v>
+      </c>
+      <c r="H6">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>35</v>
+      </c>
+      <c r="H8">
+        <v>49</v>
+      </c>
+      <c r="I8">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>